<commit_message>
Revised replication files with updated grf calibration test
</commit_message>
<xml_diff>
--- a/results/Table_A1.xlsx
+++ b/results/Table_A1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Summary Statistics of Variables in Bonn City Hall Experiment, by Participation Status</t>
   </si>
@@ -87,6 +87,9 @@
     <t>Intensity of social image concern (5 point likert scale)</t>
   </si>
   <si>
+    <t>(0.045)</t>
+  </si>
+  <si>
     <t>(0.078)</t>
   </si>
   <si>
@@ -96,6 +99,9 @@
     <t>3.750</t>
   </si>
   <si>
+    <t>(0.036)</t>
+  </si>
+  <si>
     <t>0.519</t>
   </si>
   <si>
@@ -115,6 +121,9 @@
   </si>
   <si>
     <t>3.443</t>
+  </si>
+  <si>
+    <t>(0.039)</t>
   </si>
   <si>
     <t>N</t>
@@ -217,7 +226,7 @@
         <v>1.6169454556099999e-41</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
@@ -231,7 +240,7 @@
         <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -254,7 +263,7 @@
         <v>0.0276689934596074</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
@@ -268,7 +277,7 @@
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
@@ -291,7 +300,7 @@
         <v>1.5997360565100001e-36</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
@@ -305,7 +314,7 @@
         <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
@@ -328,7 +337,7 @@
         <v>0.0034041136387086002</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13">
@@ -342,7 +351,7 @@
         <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
@@ -362,26 +371,26 @@
         <v>0.82943147581148369</v>
       </c>
       <c r="G14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B17">
         <v>614</v>
@@ -393,7 +402,7 @@
         <v>264</v>
       </c>
       <c r="G17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>